<commit_message>
Additions to final manuscript
</commit_message>
<xml_diff>
--- a/keys_coded_output.xlsx
+++ b/keys_coded_output.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -506,7 +506,7 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>has_cv2</t>
+          <t>has_cns</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -518,166 +518,154 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>has_cns</t>
+          <t>has_opiate</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>0 = no CNS disease, 1 = has some CNS disease</t>
+          <t>0 = no opiate, 1 = on opiates</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>has_opiate</t>
+          <t>AHI</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>0 = no opiate, 1 = on opiates</t>
+          <t>no coding</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>AHI</t>
+          <t>has_hfref</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>no coding</t>
+          <t>0 = no hfref, 1 = has hfref</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>has_hfref</t>
+          <t>has_hfpef_and_af</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>0 = no hfref, 1 = has hfref</t>
+          <t>0 = no hfpef or no afib, 1 = has both hfpef and af</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>has_hfpef_and_af</t>
+          <t>has_hfref_and_af</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>0 = no hfpef or no afib, 1 = has both hfpef and af</t>
+          <t>0 = no hfref or no afib, 1 = has both hfref and af</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>has_hfref_and_af</t>
+          <t>has_cva</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>0 = no hfref or no afib, 1 = has both hfref and af</t>
+          <t>0 = no cva, 1 = has had a cva</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>has_cva</t>
+          <t>has_dem_or_neurodegen</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>0 = no cva, 1 = has had a cva</t>
+          <t>0 = no dementia or neurodegen, 1 = has dementia or neurodegen</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>has_dem_or_neurodegen</t>
+          <t>has_neurodegen_and_cva</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>0 = no dementia or neurodegen, 1 = has dementia or neurodegen</t>
+          <t>0 = no cva or no neurodegen, 1 = has both cva and neurodegen</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>has_neurodegen_and_cva</t>
+          <t>has_dem_and_cva</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>0 = no cva or no neurodegen, 1 = has both cva and neurodegen</t>
+          <t>0 = no cva or no dementia, 1 = has both cva and dementia</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>has_dem_and_cva</t>
+          <t>has_dem_and_cva_or_degen</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>0 = no cva or no dementia, 1 = has both cva and dementia</t>
+          <t>1 = has (dem and cva) or (neurodegen and cva), 0 = doesn't have those combos</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>has_dem_and_cva_or_degen</t>
+          <t>FinalTx_coll</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>1 = has (dem and cva) or (neurodegen and cva), 0 = doesn't have those combos</t>
+          <t xml:space="preserve">0 = BPAP,  1 = ASV,  2 = CPAP,  3 = Other,  </t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>FinalTx</t>
+          <t>PercOSA</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t xml:space="preserve">0 = O2,  1 = asv,  2 = bipap,  3 = bipap-o2,  4 = cpap,  5 = mad,  6 = niv,  7 = niv-o2,  8 = none,  </t>
+          <t xml:space="preserve">0 = mostly_OSA,  1 = mostly_CSA,  </t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>PercOSA</t>
+          <t>StudyType</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0 = Combined OSA/CSA,  1 = Mainly OSA,  2 = Predominantly CSA,  3 = Pure CSA,  </t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="1" t="inlineStr">
-        <is>
-          <t>StudyType</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
         <is>
           <t xml:space="preserve">0 = hst,  1 = psg,  </t>
         </is>

</xml_diff>